<commit_message>
added files for all chromosomes
</commit_message>
<xml_diff>
--- a/GraphsMyUniq.xlsx
+++ b/GraphsMyUniq.xlsx
@@ -77,6 +77,35 @@
   <c:style val="44"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Exon Palindrome Count</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Chromosome</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t>s 11/14-18</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
     </c:title>
     <c:plotArea>
@@ -153,11 +182,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50113920"/>
-        <c:axId val="92275840"/>
+        <c:axId val="90657536"/>
+        <c:axId val="90659072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50113920"/>
+        <c:axId val="90657536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -165,14 +194,14 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="92275840"/>
+        <c:crossAx val="90659072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92275840"/>
+        <c:axId val="90659072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -180,7 +209,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50113920"/>
+        <c:crossAx val="90657536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -195,7 +224,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -207,6 +236,30 @@
   <c:style val="48"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Intron Palindrome Count</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Chromosomes 11/14-18</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
     </c:title>
     <c:plotArea>
@@ -283,11 +336,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="92150400"/>
-        <c:axId val="92201728"/>
+        <c:axId val="90672512"/>
+        <c:axId val="90694784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="92150400"/>
+        <c:axId val="90672512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -295,14 +348,14 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="92201728"/>
+        <c:crossAx val="90694784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92201728"/>
+        <c:axId val="90694784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -310,7 +363,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92150400"/>
+        <c:crossAx val="90672512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -325,7 +378,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -683,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>